<commit_message>
Validacion de tolvas listo
</commit_message>
<xml_diff>
--- a/Solución/Diseño Mecánico/Esclusas/Calculo de tolvas.xlsx
+++ b/Solución/Diseño Mecánico/Esclusas/Calculo de tolvas.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Cálculo por volumen" sheetId="1" r:id="rId1"/>
@@ -497,11 +497,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="8" max="8" width="13.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
@@ -527,7 +530,7 @@
         <v>3</v>
       </c>
       <c r="G3">
-        <v>20.800976813898384</v>
+        <v>16.4603868474641</v>
       </c>
       <c r="H3" t="s">
         <v>3</v>
@@ -549,7 +552,7 @@
         <v>2</v>
       </c>
       <c r="G5">
-        <v>11295</v>
+        <v>5597</v>
       </c>
       <c r="H5" t="s">
         <v>2</v>
@@ -603,7 +606,7 @@
         <v>3</v>
       </c>
       <c r="G10">
-        <v>12.919861375235483</v>
+        <v>10.223842762403184</v>
       </c>
       <c r="H10" t="s">
         <v>3</v>
@@ -617,7 +620,7 @@
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="G12">
         <f>G3/G10</f>
-        <v>1.6099999999821404</v>
+        <v>1.6099999999995085</v>
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
@@ -665,19 +668,19 @@
       </c>
       <c r="G14">
         <f>G10^2</f>
-        <v>166.9228179553017</v>
+        <v>104.52696083034395</v>
       </c>
       <c r="H14">
         <f>(2*G3*TAN(G8)+G10)^2</f>
-        <v>1044.5288106423448</v>
+        <v>654.08326683550547</v>
       </c>
       <c r="I14">
         <f>(G14+H14+SQRT(G14*H14))*(G3/3)</f>
-        <v>11295.005549895153</v>
+        <v>5597.0008377049635</v>
       </c>
       <c r="J14">
         <f>G5-I14</f>
-        <v>-5.5498951533081708E-3</v>
+        <v>-8.3770496348734014E-4</v>
       </c>
     </row>
   </sheetData>
@@ -690,8 +693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -730,15 +733,15 @@
       </c>
       <c r="D3">
         <f>-(4*A9*A5*A13)/(A11)</f>
-        <v>-0.25744443567067832</v>
+        <v>-0.25744443567178849</v>
       </c>
       <c r="E3">
         <f>1-EXP(D3)</f>
-        <v>0.22697542228760081</v>
+        <v>0.22697542228845902</v>
       </c>
       <c r="F3">
         <f>(A3*A7*A11)/(4*A5*A13)</f>
-        <v>4185.9467017661436</v>
+        <v>3312.4551144926168</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -763,7 +766,7 @@
       </c>
       <c r="D6">
         <f>E3*F3</f>
-        <v>950.10702030676032</v>
+        <v>751.8458984235275</v>
       </c>
       <c r="E6" t="s">
         <v>36</v>
@@ -786,7 +789,7 @@
       </c>
       <c r="D8">
         <f>D6*A15^2</f>
-        <v>15.859454118871952</v>
+        <v>7.8588166774970825</v>
       </c>
       <c r="E8" t="s">
         <v>35</v>
@@ -795,14 +798,14 @@
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <f>'Cálculo por volumen'!G3/100</f>
-        <v>0.20800976813898384</v>
+        <v>0.16460386847464101</v>
       </c>
       <c r="B9" t="s">
         <v>23</v>
       </c>
       <c r="D9">
         <f>D8/9.81</f>
-        <v>1.6166619896913303</v>
+        <v>0.80110261748186362</v>
       </c>
       <c r="E9" t="s">
         <v>37</v>
@@ -819,14 +822,14 @@
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <f>('Cálculo por volumen'!G10+2*'Cálculo por volumen'!G3*TAN('Cálculo por volumen'!G8))/100</f>
-        <v>0.3231917094608624</v>
+        <v>0.25575051648735836</v>
       </c>
       <c r="B11" t="s">
         <v>23</v>
       </c>
       <c r="C11">
         <f>A11</f>
-        <v>0.3231917094608624</v>
+        <v>0.25575051648735836</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -850,7 +853,7 @@
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <f>'Cálculo por volumen'!G10/100</f>
-        <v>0.12919861375235484</v>
+        <v>0.10223842762403183</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Avance 2 Oct 2018
</commit_message>
<xml_diff>
--- a/Solución/Diseño Mecánico/Esclusas/Calculo de tolvas.xlsx
+++ b/Solución/Diseño Mecánico/Esclusas/Calculo de tolvas.xlsx
@@ -4,45 +4,135 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Cálculo por volumen" sheetId="1" r:id="rId1"/>
     <sheet name="Cálculo de fuerza" sheetId="2" r:id="rId2"/>
+    <sheet name="Calculo tolva romana" sheetId="3" r:id="rId3"/>
+    <sheet name="Cálculo contenedor" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
+    <definedName name="solver_adj" localSheetId="3" hidden="1">'Cálculo contenedor'!$A$11,'Cálculo contenedor'!$B$11,'Cálculo contenedor'!$C$11</definedName>
     <definedName name="solver_adj" localSheetId="0" hidden="1">'Cálculo por volumen'!$G$3,'Cálculo por volumen'!$G$10</definedName>
+    <definedName name="solver_adj" localSheetId="2" hidden="1">'Calculo tolva romana'!$A$30,'Calculo tolva romana'!$B$30</definedName>
+    <definedName name="solver_cvg" localSheetId="3" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
+    <definedName name="solver_cvg" localSheetId="2" hidden="1">0.0001</definedName>
+    <definedName name="solver_drv" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_drv" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_itr" localSheetId="3" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_itr" localSheetId="2" hidden="1">2147483647</definedName>
+    <definedName name="solver_lhs1" localSheetId="3" hidden="1">'Cálculo contenedor'!$A$11</definedName>
     <definedName name="solver_lhs1" localSheetId="0" hidden="1">'Cálculo por volumen'!$G$12</definedName>
+    <definedName name="solver_lhs1" localSheetId="2" hidden="1">'Calculo tolva romana'!$A$30</definedName>
+    <definedName name="solver_lhs2" localSheetId="3" hidden="1">'Cálculo contenedor'!$B$11</definedName>
+    <definedName name="solver_lhs2" localSheetId="2" hidden="1">'Calculo tolva romana'!$B$30</definedName>
+    <definedName name="solver_lhs3" localSheetId="3" hidden="1">'Cálculo contenedor'!$B$15</definedName>
+    <definedName name="solver_lhs3" localSheetId="2" hidden="1">'Calculo tolva romana'!$B$37</definedName>
+    <definedName name="solver_lhs4" localSheetId="3" hidden="1">'Cálculo contenedor'!$B$18</definedName>
+    <definedName name="solver_lhs4" localSheetId="2" hidden="1">'Calculo tolva romana'!$C$11</definedName>
+    <definedName name="solver_lhs5" localSheetId="3" hidden="1">'Cálculo contenedor'!$C$11</definedName>
+    <definedName name="solver_lhs5" localSheetId="2" hidden="1">'Calculo tolva romana'!$D$11</definedName>
+    <definedName name="solver_lhs6" localSheetId="2" hidden="1">'Calculo tolva romana'!$G$11</definedName>
+    <definedName name="solver_mip" localSheetId="3" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="2" hidden="1">2147483647</definedName>
+    <definedName name="solver_mni" localSheetId="3" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
+    <definedName name="solver_mni" localSheetId="2" hidden="1">30</definedName>
+    <definedName name="solver_mrt" localSheetId="3" hidden="1">0.075</definedName>
     <definedName name="solver_mrt" localSheetId="0" hidden="1">0.075</definedName>
+    <definedName name="solver_mrt" localSheetId="2" hidden="1">0.075</definedName>
+    <definedName name="solver_msl" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_msl" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_msl" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_neg" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_nod" localSheetId="3" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_nod" localSheetId="2" hidden="1">2147483647</definedName>
+    <definedName name="solver_num" localSheetId="3" hidden="1">5</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_num" localSheetId="2" hidden="1">3</definedName>
+    <definedName name="solver_nwt" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_nwt" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_opt" localSheetId="3" hidden="1">'Cálculo contenedor'!$B$21</definedName>
     <definedName name="solver_opt" localSheetId="0" hidden="1">'Cálculo por volumen'!$J$14</definedName>
+    <definedName name="solver_opt" localSheetId="2" hidden="1">'Calculo tolva romana'!$B$34</definedName>
+    <definedName name="solver_pre" localSheetId="3" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
+    <definedName name="solver_pre" localSheetId="2" hidden="1">0.000001</definedName>
+    <definedName name="solver_rbv" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rbv" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_rel1" localSheetId="3" hidden="1">3</definedName>
     <definedName name="solver_rel1" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rel1" localSheetId="2" hidden="1">3</definedName>
+    <definedName name="solver_rel2" localSheetId="3" hidden="1">3</definedName>
+    <definedName name="solver_rel2" localSheetId="2" hidden="1">3</definedName>
+    <definedName name="solver_rel3" localSheetId="3" hidden="1">2</definedName>
+    <definedName name="solver_rel3" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_rel4" localSheetId="3" hidden="1">2</definedName>
+    <definedName name="solver_rel4" localSheetId="2" hidden="1">3</definedName>
+    <definedName name="solver_rel5" localSheetId="3" hidden="1">3</definedName>
+    <definedName name="solver_rel5" localSheetId="2" hidden="1">3</definedName>
+    <definedName name="solver_rel6" localSheetId="2" hidden="1">3</definedName>
+    <definedName name="solver_rhs1" localSheetId="3" hidden="1">0</definedName>
     <definedName name="solver_rhs1" localSheetId="0" hidden="1">1.61</definedName>
+    <definedName name="solver_rhs1" localSheetId="2" hidden="1">0</definedName>
+    <definedName name="solver_rhs2" localSheetId="3" hidden="1">0</definedName>
+    <definedName name="solver_rhs2" localSheetId="2" hidden="1">0</definedName>
+    <definedName name="solver_rhs3" localSheetId="3" hidden="1">0</definedName>
+    <definedName name="solver_rhs3" localSheetId="2" hidden="1">0</definedName>
+    <definedName name="solver_rhs4" localSheetId="3" hidden="1">0</definedName>
+    <definedName name="solver_rhs4" localSheetId="2" hidden="1">0</definedName>
+    <definedName name="solver_rhs5" localSheetId="3" hidden="1">30</definedName>
+    <definedName name="solver_rhs5" localSheetId="2" hidden="1">0</definedName>
+    <definedName name="solver_rhs6" localSheetId="2" hidden="1">0</definedName>
+    <definedName name="solver_rlx" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rlx" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_rsd" localSheetId="3" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_rsd" localSheetId="2" hidden="1">0</definedName>
+    <definedName name="solver_scl" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_scl" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_scl" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_sho" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_ssz" localSheetId="3" hidden="1">100</definedName>
     <definedName name="solver_ssz" localSheetId="0" hidden="1">100</definedName>
+    <definedName name="solver_ssz" localSheetId="2" hidden="1">100</definedName>
+    <definedName name="solver_tim" localSheetId="3" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_tim" localSheetId="2" hidden="1">2147483647</definedName>
+    <definedName name="solver_tol" localSheetId="3" hidden="1">0.01</definedName>
     <definedName name="solver_tol" localSheetId="0" hidden="1">0.01</definedName>
+    <definedName name="solver_tol" localSheetId="2" hidden="1">0.01</definedName>
+    <definedName name="solver_typ" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_typ" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_typ" localSheetId="2" hidden="1">3</definedName>
+    <definedName name="solver_val" localSheetId="3" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_val" localSheetId="2" hidden="1">0</definedName>
+    <definedName name="solver_ver" localSheetId="3" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_ver" localSheetId="2" hidden="1">3</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -52,7 +142,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="67">
   <si>
     <t>Altura deseada</t>
   </si>
@@ -169,13 +259,97 @@
   </si>
   <si>
     <t>Razon aurea</t>
+  </si>
+  <si>
+    <t>Determinación de volumen de la tolva romana</t>
+  </si>
+  <si>
+    <t>En esta hoja se intentó determinar el tamaño de la tolva romana, sujeto a 7 ecuaciones contemplando el factor de seguridad.</t>
+  </si>
+  <si>
+    <t>Los cálculos previos están en la hoja del 1 de Octubre, consecutivo 5.</t>
+  </si>
+  <si>
+    <t>Ecuación 1</t>
+  </si>
+  <si>
+    <t>Ecuación 2</t>
+  </si>
+  <si>
+    <t>Ecuación 3</t>
+  </si>
+  <si>
+    <t>Factor de seguridad</t>
+  </si>
+  <si>
+    <t>Parámetros a encontrar</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>Volumen cubo</t>
+  </si>
+  <si>
+    <t>Area Mayor</t>
+  </si>
+  <si>
+    <t>Area Menor</t>
+  </si>
+  <si>
+    <t>Volumen pirámide</t>
+  </si>
+  <si>
+    <t>Objetivo</t>
+  </si>
+  <si>
+    <t>Determinación de volumen de los contenedores</t>
+  </si>
+  <si>
+    <t>En esta hoja se intentó determinar el tamaño de los contenedores para cada alimento sujeto a 3 ecuaciones contemplando el factor de seguridad.</t>
+  </si>
+  <si>
+    <t>Los cálculos previos están en la hoja del 1 de Octubre, consecutivo 6.</t>
+  </si>
+  <si>
+    <t>Concentrado</t>
+  </si>
+  <si>
+    <t>Volumen cilindro</t>
+  </si>
+  <si>
+    <t>CitroCon</t>
+  </si>
+  <si>
+    <t>Mineral</t>
+  </si>
+  <si>
+    <t>Levadura</t>
+  </si>
+  <si>
+    <t>Tolva general</t>
+  </si>
+  <si>
+    <t>Tolva mineral</t>
+  </si>
+  <si>
+    <t>Tolva Levadura</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -187,6 +361,21 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -212,9 +401,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -498,7 +690,7 @@
   <dimension ref="B1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -693,7 +885,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -859,4 +1051,1032 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K37"/>
+  <sheetViews>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" t="s">
+        <v>1</v>
+      </c>
+      <c r="I6" t="s">
+        <v>45</v>
+      </c>
+      <c r="K6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>13939</v>
+      </c>
+      <c r="B7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>1.3</v>
+      </c>
+      <c r="E7">
+        <f>A7*C7</f>
+        <v>18120.7</v>
+      </c>
+      <c r="G7">
+        <v>160.6</v>
+      </c>
+      <c r="H7" t="s">
+        <v>2</v>
+      </c>
+      <c r="I7">
+        <v>1.3</v>
+      </c>
+      <c r="K7">
+        <f>G7*I7</f>
+        <v>208.78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>46</v>
+      </c>
+      <c r="G9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" t="s">
+        <v>50</v>
+      </c>
+      <c r="G10" t="s">
+        <v>47</v>
+      </c>
+      <c r="H10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>41.470457973748012</v>
+      </c>
+      <c r="B11">
+        <v>20.739221383930818</v>
+      </c>
+      <c r="C11">
+        <v>12.426939674491317</v>
+      </c>
+      <c r="D11">
+        <v>10.369610691965407</v>
+      </c>
+      <c r="G11">
+        <v>5.050985283431098</v>
+      </c>
+      <c r="H11">
+        <v>8.1825961591545759</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" t="s">
+        <v>54</v>
+      </c>
+      <c r="G13" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f>C11*C11*D11</f>
+        <v>1601.366843329474</v>
+      </c>
+      <c r="B14">
+        <f>(A11*A11)</f>
+        <v>1719.7988845524001</v>
+      </c>
+      <c r="C14">
+        <f>C11*C11</f>
+        <v>154.42882967344636</v>
+      </c>
+      <c r="D14">
+        <f>(B11/3)*(B14+C14+SQRT(B14*C14))</f>
+        <v>16519.333156619374</v>
+      </c>
+      <c r="G14">
+        <f>G11*G11*H11</f>
+        <v>208.75809447420013</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15">
+        <f>E7-D14-A14</f>
+        <v>5.1152937885490246E-8</v>
+      </c>
+      <c r="G15" t="s">
+        <v>55</v>
+      </c>
+      <c r="H15">
+        <f>K7-J14-G14</f>
+        <v>2.1905525799866155E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>55</v>
+      </c>
+      <c r="B18">
+        <f>2*B11*TAN(35*PI()/180)+C11-A11</f>
+        <v>0</v>
+      </c>
+      <c r="G18" t="s">
+        <v>55</v>
+      </c>
+      <c r="H18">
+        <f>1.62*G11-H11</f>
+        <v>3.8031799931559362E-12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>55</v>
+      </c>
+      <c r="B21">
+        <f>2*D11-B11</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25" t="s">
+        <v>45</v>
+      </c>
+      <c r="E25" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>28.16</v>
+      </c>
+      <c r="B26" t="s">
+        <v>2</v>
+      </c>
+      <c r="C26">
+        <v>1.3</v>
+      </c>
+      <c r="E26">
+        <f>A26*C26</f>
+        <v>36.608000000000004</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>47</v>
+      </c>
+      <c r="B29" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>2.8271785049016125</v>
+      </c>
+      <c r="B30">
+        <v>4.5800291779406122</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <f>A30*A30*B30</f>
+        <v>36.607890624964938</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>55</v>
+      </c>
+      <c r="B34">
+        <f>E26-D33-A33</f>
+        <v>1.0937503506625035E-4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>55</v>
+      </c>
+      <c r="B37">
+        <f>1.62*A30-B30</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q40"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>59</v>
+      </c>
+      <c r="G5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K6" t="s">
+        <v>11</v>
+      </c>
+      <c r="M6" t="s">
+        <v>1</v>
+      </c>
+      <c r="O6" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f>E7/C7</f>
+        <v>253376.92307692306</v>
+      </c>
+      <c r="B7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>1.3</v>
+      </c>
+      <c r="E7">
+        <v>329390</v>
+      </c>
+      <c r="G7">
+        <f>K7/I7</f>
+        <v>163284.61538461538</v>
+      </c>
+      <c r="H7" t="s">
+        <v>2</v>
+      </c>
+      <c r="I7">
+        <v>1.3</v>
+      </c>
+      <c r="K7">
+        <v>212270</v>
+      </c>
+      <c r="M7">
+        <v>704.7</v>
+      </c>
+      <c r="N7" t="s">
+        <v>2</v>
+      </c>
+      <c r="O7">
+        <v>1.3</v>
+      </c>
+      <c r="Q7">
+        <v>329390</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>46</v>
+      </c>
+      <c r="G9" t="s">
+        <v>46</v>
+      </c>
+      <c r="M9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" t="s">
+        <v>50</v>
+      </c>
+      <c r="G10" t="s">
+        <v>47</v>
+      </c>
+      <c r="H10" t="s">
+        <v>48</v>
+      </c>
+      <c r="I10" t="s">
+        <v>49</v>
+      </c>
+      <c r="J10" t="s">
+        <v>50</v>
+      </c>
+      <c r="M10" t="s">
+        <v>47</v>
+      </c>
+      <c r="N10" t="s">
+        <v>48</v>
+      </c>
+      <c r="O10" t="s">
+        <v>49</v>
+      </c>
+      <c r="P10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>92.040498261833122</v>
+      </c>
+      <c r="B11">
+        <v>41.020249130916532</v>
+      </c>
+      <c r="C11">
+        <v>30</v>
+      </c>
+      <c r="D11">
+        <v>10</v>
+      </c>
+      <c r="G11">
+        <v>66.952783668144292</v>
+      </c>
+      <c r="H11">
+        <v>28.476391834072121</v>
+      </c>
+      <c r="I11">
+        <v>46.131754771196874</v>
+      </c>
+      <c r="J11">
+        <v>10</v>
+      </c>
+      <c r="M11">
+        <v>77.056553466484701</v>
+      </c>
+      <c r="N11">
+        <v>33.528276733242038</v>
+      </c>
+      <c r="O11">
+        <v>54.315808307852151</v>
+      </c>
+      <c r="P11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>42</v>
+      </c>
+      <c r="G12" t="s">
+        <v>42</v>
+      </c>
+      <c r="M12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>60</v>
+      </c>
+      <c r="B13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" t="s">
+        <v>54</v>
+      </c>
+      <c r="G13" t="s">
+        <v>60</v>
+      </c>
+      <c r="H13" t="s">
+        <v>52</v>
+      </c>
+      <c r="I13" t="s">
+        <v>53</v>
+      </c>
+      <c r="J13" t="s">
+        <v>54</v>
+      </c>
+      <c r="M13" t="s">
+        <v>60</v>
+      </c>
+      <c r="N13" t="s">
+        <v>52</v>
+      </c>
+      <c r="O13" t="s">
+        <v>53</v>
+      </c>
+      <c r="P13" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f>PI()/4*A11^2*C11</f>
+        <v>199603.91637180711</v>
+      </c>
+      <c r="B14">
+        <f>(A11*A11)</f>
+        <v>8471.4533202865059</v>
+      </c>
+      <c r="C14">
+        <f>D11*D11</f>
+        <v>100</v>
+      </c>
+      <c r="D14" s="4">
+        <f>(B11/3)*(B14+C14+SQRT(B14*C14))</f>
+        <v>129786.13076683834</v>
+      </c>
+      <c r="G14">
+        <f>PI()/4*G11^2*I11</f>
+        <v>162415.37249437472</v>
+      </c>
+      <c r="H14">
+        <f>(G11*G11)</f>
+        <v>4482.6752409133287</v>
+      </c>
+      <c r="I14">
+        <f>J11*J11</f>
+        <v>100</v>
+      </c>
+      <c r="J14">
+        <f>(H11/3)*(H14+I14+SQRT(H14*I14))</f>
+        <v>49854.597609902732</v>
+      </c>
+      <c r="M14">
+        <f>PI()/4*M11^2*O11</f>
+        <v>253300.05778133572</v>
+      </c>
+      <c r="N14">
+        <f>(M11*M11)</f>
+        <v>5937.7124321332158</v>
+      </c>
+      <c r="O14">
+        <f>P11*P11</f>
+        <v>100</v>
+      </c>
+      <c r="P14">
+        <f>(N11/3)*(N14+O14+SQRT(N14*O14))</f>
+        <v>76089.942582546646</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15">
+        <f>E7-D14-A14</f>
+        <v>-4.7138645430095494E-2</v>
+      </c>
+      <c r="G15" t="s">
+        <v>55</v>
+      </c>
+      <c r="H15">
+        <f>K7-J14-G14</f>
+        <v>2.9895722545916215E-2</v>
+      </c>
+      <c r="M15" t="s">
+        <v>55</v>
+      </c>
+      <c r="N15">
+        <f>Q7-P14-M14</f>
+        <v>-3.6388236912898719E-4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>43</v>
+      </c>
+      <c r="G17" t="s">
+        <v>43</v>
+      </c>
+      <c r="M17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>55</v>
+      </c>
+      <c r="B18">
+        <f>2*B11*TAN(45*PI()/180)+D11-A11</f>
+        <v>0</v>
+      </c>
+      <c r="G18" t="s">
+        <v>55</v>
+      </c>
+      <c r="H18">
+        <f>2*H11*TAN(45*PI()/180)+J11-G11</f>
+        <v>0</v>
+      </c>
+      <c r="M18" t="s">
+        <v>55</v>
+      </c>
+      <c r="N18">
+        <f>2*N11*TAN(45*PI()/180)+P11-M11</f>
+        <v>-6.3948846218409017E-13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>44</v>
+      </c>
+      <c r="G20" t="s">
+        <v>44</v>
+      </c>
+      <c r="M20" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>55</v>
+      </c>
+      <c r="B21">
+        <f>B11+C11</f>
+        <v>71.02024913091654</v>
+      </c>
+      <c r="G21" t="s">
+        <v>55</v>
+      </c>
+      <c r="H21">
+        <f>1.62*H11-I11</f>
+        <v>0</v>
+      </c>
+      <c r="M21" t="s">
+        <v>55</v>
+      </c>
+      <c r="N21">
+        <f>1.62*N11-O11</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>62</v>
+      </c>
+      <c r="G24" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E25" t="s">
+        <v>11</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J25" s="2"/>
+      <c r="K25" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>253380</v>
+      </c>
+      <c r="B26" t="s">
+        <v>2</v>
+      </c>
+      <c r="C26">
+        <v>1.3</v>
+      </c>
+      <c r="E26">
+        <f>A26*C26</f>
+        <v>329394</v>
+      </c>
+      <c r="G26">
+        <v>704.7</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I26" s="3">
+        <v>1.3</v>
+      </c>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3">
+        <f>G26*I26</f>
+        <v>916.11000000000013</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>46</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>47</v>
+      </c>
+      <c r="B29" t="s">
+        <v>48</v>
+      </c>
+      <c r="C29" t="s">
+        <v>49</v>
+      </c>
+      <c r="D29" t="s">
+        <v>50</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="I29" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="J29" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="K29" s="3"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>41.470457973748012</v>
+      </c>
+      <c r="B30">
+        <v>20.739221383930818</v>
+      </c>
+      <c r="C30">
+        <v>12.426939674491317</v>
+      </c>
+      <c r="D30">
+        <v>4</v>
+      </c>
+      <c r="G30">
+        <v>10.515515089146165</v>
+      </c>
+      <c r="H30">
+        <v>4.6525599437313581</v>
+      </c>
+      <c r="I30">
+        <v>7.5371471088447999</v>
+      </c>
+      <c r="J30">
+        <v>4</v>
+      </c>
+      <c r="K30" s="3"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>42</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="3"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>60</v>
+      </c>
+      <c r="B32" t="s">
+        <v>52</v>
+      </c>
+      <c r="C32" t="s">
+        <v>53</v>
+      </c>
+      <c r="D32" t="s">
+        <v>54</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I32" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J32" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="K32" s="3"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <f>PI()/4*A30^2*C30</f>
+        <v>16785.401520839139</v>
+      </c>
+      <c r="B33">
+        <f>(A30*A30)</f>
+        <v>1719.7988845524001</v>
+      </c>
+      <c r="C33">
+        <f>D30*D30</f>
+        <v>16</v>
+      </c>
+      <c r="D33">
+        <f>(B30/3)*(B33+C33+SQRT(B33*C33))</f>
+        <v>13146.459126651544</v>
+      </c>
+      <c r="G33" s="3">
+        <f>PI()/4*G30^2*I30</f>
+        <v>654.5728305554137</v>
+      </c>
+      <c r="H33" s="3">
+        <f>(G30*G30)</f>
+        <v>110.57605759006067</v>
+      </c>
+      <c r="I33" s="3">
+        <f>J30*J30</f>
+        <v>16</v>
+      </c>
+      <c r="J33" s="3">
+        <f>(H30/3)*(H33+I33+SQRT(H33*I33))</f>
+        <v>261.5329841816021</v>
+      </c>
+      <c r="K33" s="3"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>55</v>
+      </c>
+      <c r="B34">
+        <f>E26-D33-A33</f>
+        <v>299462.13935250934</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H34" s="3">
+        <f>K26-J33-G33</f>
+        <v>4.1852629842651368E-3</v>
+      </c>
+      <c r="I34" s="3"/>
+      <c r="J34" s="3"/>
+      <c r="K34" s="3"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="3"/>
+      <c r="J35" s="3"/>
+      <c r="K35" s="3"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>43</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H36" s="3"/>
+      <c r="I36" s="3"/>
+      <c r="J36" s="3"/>
+      <c r="K36" s="3"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>55</v>
+      </c>
+      <c r="B37">
+        <f>2*B30*TAN(35*PI()/180)+D30-A30</f>
+        <v>-8.4269396744912797</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H37" s="3">
+        <f>2*H30*TAN(35*PI()/180)+J30-G30</f>
+        <v>3.1441516057384433E-13</v>
+      </c>
+      <c r="I37" s="3"/>
+      <c r="J37" s="3"/>
+      <c r="K37" s="3"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G38" s="3"/>
+      <c r="H38" s="3"/>
+      <c r="I38" s="3"/>
+      <c r="J38" s="3"/>
+      <c r="K38" s="3"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>44</v>
+      </c>
+      <c r="G39" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H39" s="3"/>
+      <c r="I39" s="3"/>
+      <c r="J39" s="3"/>
+      <c r="K39" s="3"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>55</v>
+      </c>
+      <c r="B40">
+        <f>1.62*B30-C30</f>
+        <v>21.170598967476614</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H40" s="3">
+        <f>1.62*H30-I30</f>
+        <v>0</v>
+      </c>
+      <c r="I40" s="3"/>
+      <c r="J40" s="3"/>
+      <c r="K40" s="3"/>
+    </row>
+  </sheetData>
+  <scenarios current="2">
+    <scenario name="Adicional" count="3" user="Autor" comment="Creado por Autor el 10/1/2018">
+      <inputCells r="A11" val="48.374112909098"/>
+      <inputCells r="B11" val="31.6864004510389"/>
+      <inputCells r="C11" val="51.331968730683"/>
+    </scenario>
+    <scenario name="Mineral" count="3" user="Autor" comment="Creado por Autor el 10/1/2018">
+      <inputCells r="A11" val="29.5979086817967"/>
+      <inputCells r="B11" val="18.2788011303374"/>
+      <inputCells r="C11" val="29.6116578311466"/>
+    </scenario>
+    <scenario name="Levadura" count="3" user="Autor" comment="Creado por Autor el 10/1/2018">
+      <inputCells r="A11" val="10.5155150891462"/>
+      <inputCells r="B11" val="4.65255994373136"/>
+      <inputCells r="C11" val="7.5371471088448"/>
+    </scenario>
+  </scenarios>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Avance 11-3 Laimi 1
</commit_message>
<xml_diff>
--- a/Solución/Diseño Mecánico/Esclusas/Calculo de tolvas.xlsx
+++ b/Solución/Diseño Mecánico/Esclusas/Calculo de tolvas.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Cálculo contenedor Concentrado" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="solver_adj" localSheetId="5" hidden="1">'Cálculo contenedor'!$A$11,'Cálculo contenedor'!$B$11,'Cálculo contenedor'!$C$11</definedName>
-    <definedName name="solver_adj" localSheetId="1" hidden="1">'Cálculo contenedor CC'!$W$15:$X$15</definedName>
+    <definedName name="solver_adj" localSheetId="1" hidden="1">'Cálculo contenedor CC'!$W$15:$Y$15</definedName>
     <definedName name="solver_adj" localSheetId="0" hidden="1">'Cálculo contenedor Concentrado'!$W$15:$Y$15</definedName>
     <definedName name="solver_adj" localSheetId="3" hidden="1">'Calculo tolva romana'!$S$26,'Calculo tolva romana'!$U$26,'Calculo tolva romana'!$V$26</definedName>
     <definedName name="solver_adj" localSheetId="7" hidden="1">'Dimensionado tolva levadura'!$I$15:$J$15</definedName>
@@ -1491,8 +1491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="X20" sqref="X20"/>
+    <sheetView topLeftCell="N1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="Z25" sqref="Z25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1500,7 +1500,8 @@
     <col min="1" max="1" width="10.7109375" hidden="1" customWidth="1"/>
     <col min="2" max="7" width="0" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="13.7109375" hidden="1" customWidth="1"/>
-    <col min="9" max="14" width="0" hidden="1" customWidth="1"/>
+    <col min="9" max="13" width="0" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="0.85546875" customWidth="1"/>
     <col min="15" max="15" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2199,8 +2200,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="Y15" sqref="Y15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2303,7 +2304,7 @@
       </c>
       <c r="J9">
         <f>B19/B18</f>
-        <v>338983.05084745766</v>
+        <v>400000.00000000006</v>
       </c>
       <c r="O9">
         <v>1</v>
@@ -2316,7 +2317,7 @@
       </c>
       <c r="X9">
         <f>P19/P18</f>
-        <v>467796.61016949156</v>
+        <v>400000.00000000006</v>
       </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
@@ -2357,7 +2358,7 @@
       </c>
       <c r="J11">
         <f>J9*B20</f>
-        <v>440677.96610169497</v>
+        <v>520000.00000000012</v>
       </c>
       <c r="O11">
         <v>3</v>
@@ -2370,7 +2371,7 @@
       </c>
       <c r="X11">
         <f>X9*P20</f>
-        <v>561355.93220338982</v>
+        <v>480000.00000000006</v>
       </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
@@ -2454,13 +2455,13 @@
         <v>30</v>
       </c>
       <c r="W15">
-        <v>125.13049797382367</v>
+        <v>104.14290501508998</v>
       </c>
       <c r="X15">
-        <v>101.76707645669109</v>
+        <v>83.591287790140328</v>
       </c>
       <c r="Y15">
-        <v>0</v>
+        <v>14.469266361528636</v>
       </c>
       <c r="Z15">
         <f>P17</f>
@@ -2538,7 +2539,7 @@
         <v>78</v>
       </c>
       <c r="B18">
-        <v>0.29499999999999998</v>
+        <v>0.34499999999999997</v>
       </c>
       <c r="I18">
         <f>(I15*I15)*K15</f>
@@ -2564,15 +2565,15 @@
         <v>78</v>
       </c>
       <c r="P18">
-        <v>0.29499999999999998</v>
+        <v>0.34499999999999997</v>
       </c>
       <c r="W18">
         <f>(W15*W15)*Y15</f>
-        <v>0</v>
+        <v>156929.96844675348</v>
       </c>
       <c r="X18">
         <f>(W15*W15)</f>
-        <v>15657.641523177088</v>
+        <v>10845.744664982054</v>
       </c>
       <c r="Y18">
         <f>PI()*(Z15/2)^2</f>
@@ -2580,11 +2581,11 @@
       </c>
       <c r="Z18">
         <f>(X15/3)*(X18+Y18+SQRT(X18*Y18))</f>
-        <v>561355.93220338796</v>
+        <v>323070.03155324777</v>
       </c>
       <c r="AA18">
         <f>W18+Z18</f>
-        <v>561355.93220338796</v>
+        <v>480000.00000000128</v>
       </c>
     </row>
     <row r="19" spans="1:27" x14ac:dyDescent="0.25">
@@ -2592,8 +2593,7 @@
         <v>79</v>
       </c>
       <c r="B19">
-        <f>B21*B22</f>
-        <v>100000</v>
+        <v>138000</v>
       </c>
       <c r="I19" t="s">
         <v>92</v>
@@ -2620,7 +2620,7 @@
       </c>
       <c r="J20">
         <f>J11-M18</f>
-        <v>0.34723037760704756</v>
+        <v>79322.381128682755</v>
       </c>
       <c r="O20" t="s">
         <v>83</v>
@@ -2633,7 +2633,7 @@
       </c>
       <c r="X20">
         <f>X11-AA18</f>
-        <v>1.862645149230957E-9</v>
+        <v>-1.2223608791828156E-9</v>
       </c>
     </row>
     <row r="21" spans="1:27" x14ac:dyDescent="0.25">
@@ -2707,7 +2707,7 @@
       </c>
       <c r="X26">
         <f>4*W15*Y15+4/2*(W15+Z15)*X15/COS(P16)</f>
-        <v>31199.154246354166</v>
+        <v>27602.846259270962</v>
       </c>
     </row>
     <row r="32" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3809,7 +3809,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R32"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F9" sqref="F9:F10"/>
     </sheetView>
   </sheetViews>

</xml_diff>